<commit_message>
Added missing define for wolfe
</commit_message>
<xml_diff>
--- a/doc/WOLFE_APB_SOC_CTRL_reference.xlsx
+++ b/doc/WOLFE_APB_SOC_CTRL_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IPREGLIST_rel1.0.0" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t xml:space="preserve">Register Name</t>
   </si>
@@ -68,10 +68,10 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">RTC_FIRST_REG</t>
+    <t xml:space="preserve">SLEEP_CONTROL</t>
   </si>
   <si>
-    <t xml:space="preserve">0x1D0</t>
+    <t xml:space="preserve">0x104</t>
   </si>
   <si>
     <t xml:space="preserve">Config</t>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t xml:space="preserve">0x0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep sleep control register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTC_FIRST_REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1D0</t>
   </si>
   <si>
     <t xml:space="preserve">First RTC register</t>
@@ -108,6 +117,40 @@
   </si>
   <si>
     <t xml:space="preserve">Reset Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLL_RET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLL retention configuration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEM_RET_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory retention configuration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTWAKEUP_SEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External wakeup selection. This gives the GPIO numer which can wakeup the chip when it is in deep sleep mode.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTWAKEUP_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External wakeup type. This tells the way the external GPIO can wakeup the chip while it is in deep sleep (raising edge, falling edge, etc). Possible values:
+- 0: Rising edge.
+- 1: Falling edge.
+- 2: Level high.
+- 3: Level low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTWAKEUP_EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External wakeup enable.</t>
   </si>
 </sst>
 </file>
@@ -201,7 +244,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -232,6 +275,18 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -314,26 +369,26 @@
   </sheetPr>
   <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.3117408906883"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.0485829959514"/>
     <col collapsed="false" hidden="true" max="2" min="2" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.4493927125506"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.19028340080972"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.4493927125506"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.1619433198381"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.4493927125506"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="58.5384615384615"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="10.4493927125506"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="53.8825910931174"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="2" width="10.4493927125506"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.51821862348178"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="11.085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.3400809716599"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="62.3441295546559"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="11.085020242915"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="2" width="11.085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,7 +2485,7 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -3474,9 +3529,1050 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="0"/>
+      <c r="AA4" s="0"/>
+      <c r="AB4" s="0"/>
+      <c r="AC4" s="0"/>
+      <c r="AD4" s="0"/>
+      <c r="AE4" s="0"/>
+      <c r="AF4" s="0"/>
+      <c r="AG4" s="0"/>
+      <c r="AH4" s="0"/>
+      <c r="AI4" s="0"/>
+      <c r="AJ4" s="0"/>
+      <c r="AK4" s="0"/>
+      <c r="AL4" s="0"/>
+      <c r="AM4" s="0"/>
+      <c r="AN4" s="0"/>
+      <c r="AO4" s="0"/>
+      <c r="AP4" s="0"/>
+      <c r="AQ4" s="0"/>
+      <c r="AR4" s="0"/>
+      <c r="AS4" s="0"/>
+      <c r="AT4" s="0"/>
+      <c r="AU4" s="0"/>
+      <c r="AV4" s="0"/>
+      <c r="AW4" s="0"/>
+      <c r="AX4" s="0"/>
+      <c r="AY4" s="0"/>
+      <c r="AZ4" s="0"/>
+      <c r="BA4" s="0"/>
+      <c r="BB4" s="0"/>
+      <c r="BC4" s="0"/>
+      <c r="BD4" s="0"/>
+      <c r="BE4" s="0"/>
+      <c r="BF4" s="0"/>
+      <c r="BG4" s="0"/>
+      <c r="BH4" s="0"/>
+      <c r="BI4" s="0"/>
+      <c r="BJ4" s="0"/>
+      <c r="BK4" s="0"/>
+      <c r="BL4" s="0"/>
+      <c r="BM4" s="0"/>
+      <c r="BN4" s="0"/>
+      <c r="BO4" s="0"/>
+      <c r="BP4" s="0"/>
+      <c r="BQ4" s="0"/>
+      <c r="BR4" s="0"/>
+      <c r="BS4" s="0"/>
+      <c r="BT4" s="0"/>
+      <c r="BU4" s="0"/>
+      <c r="BV4" s="0"/>
+      <c r="BW4" s="0"/>
+      <c r="BX4" s="0"/>
+      <c r="BY4" s="0"/>
+      <c r="BZ4" s="0"/>
+      <c r="CA4" s="0"/>
+      <c r="CB4" s="0"/>
+      <c r="CC4" s="0"/>
+      <c r="CD4" s="0"/>
+      <c r="CE4" s="0"/>
+      <c r="CF4" s="0"/>
+      <c r="CG4" s="0"/>
+      <c r="CH4" s="0"/>
+      <c r="CI4" s="0"/>
+      <c r="CJ4" s="0"/>
+      <c r="CK4" s="0"/>
+      <c r="CL4" s="0"/>
+      <c r="CM4" s="0"/>
+      <c r="CN4" s="0"/>
+      <c r="CO4" s="0"/>
+      <c r="CP4" s="0"/>
+      <c r="CQ4" s="0"/>
+      <c r="CR4" s="0"/>
+      <c r="CS4" s="0"/>
+      <c r="CT4" s="0"/>
+      <c r="CU4" s="0"/>
+      <c r="CV4" s="0"/>
+      <c r="CW4" s="0"/>
+      <c r="CX4" s="0"/>
+      <c r="CY4" s="0"/>
+      <c r="CZ4" s="0"/>
+      <c r="DA4" s="0"/>
+      <c r="DB4" s="0"/>
+      <c r="DC4" s="0"/>
+      <c r="DD4" s="0"/>
+      <c r="DE4" s="0"/>
+      <c r="DF4" s="0"/>
+      <c r="DG4" s="0"/>
+      <c r="DH4" s="0"/>
+      <c r="DI4" s="0"/>
+      <c r="DJ4" s="0"/>
+      <c r="DK4" s="0"/>
+      <c r="DL4" s="0"/>
+      <c r="DM4" s="0"/>
+      <c r="DN4" s="0"/>
+      <c r="DO4" s="0"/>
+      <c r="DP4" s="0"/>
+      <c r="DQ4" s="0"/>
+      <c r="DR4" s="0"/>
+      <c r="DS4" s="0"/>
+      <c r="DT4" s="0"/>
+      <c r="DU4" s="0"/>
+      <c r="DV4" s="0"/>
+      <c r="DW4" s="0"/>
+      <c r="DX4" s="0"/>
+      <c r="DY4" s="0"/>
+      <c r="DZ4" s="0"/>
+      <c r="EA4" s="0"/>
+      <c r="EB4" s="0"/>
+      <c r="EC4" s="0"/>
+      <c r="ED4" s="0"/>
+      <c r="EE4" s="0"/>
+      <c r="EF4" s="0"/>
+      <c r="EG4" s="0"/>
+      <c r="EH4" s="0"/>
+      <c r="EI4" s="0"/>
+      <c r="EJ4" s="0"/>
+      <c r="EK4" s="0"/>
+      <c r="EL4" s="0"/>
+      <c r="EM4" s="0"/>
+      <c r="EN4" s="0"/>
+      <c r="EO4" s="0"/>
+      <c r="EP4" s="0"/>
+      <c r="EQ4" s="0"/>
+      <c r="ER4" s="0"/>
+      <c r="ES4" s="0"/>
+      <c r="ET4" s="0"/>
+      <c r="EU4" s="0"/>
+      <c r="EV4" s="0"/>
+      <c r="EW4" s="0"/>
+      <c r="EX4" s="0"/>
+      <c r="EY4" s="0"/>
+      <c r="EZ4" s="0"/>
+      <c r="FA4" s="0"/>
+      <c r="FB4" s="0"/>
+      <c r="FC4" s="0"/>
+      <c r="FD4" s="0"/>
+      <c r="FE4" s="0"/>
+      <c r="FF4" s="0"/>
+      <c r="FG4" s="0"/>
+      <c r="FH4" s="0"/>
+      <c r="FI4" s="0"/>
+      <c r="FJ4" s="0"/>
+      <c r="FK4" s="0"/>
+      <c r="FL4" s="0"/>
+      <c r="FM4" s="0"/>
+      <c r="FN4" s="0"/>
+      <c r="FO4" s="0"/>
+      <c r="FP4" s="0"/>
+      <c r="FQ4" s="0"/>
+      <c r="FR4" s="0"/>
+      <c r="FS4" s="0"/>
+      <c r="FT4" s="0"/>
+      <c r="FU4" s="0"/>
+      <c r="FV4" s="0"/>
+      <c r="FW4" s="0"/>
+      <c r="FX4" s="0"/>
+      <c r="FY4" s="0"/>
+      <c r="FZ4" s="0"/>
+      <c r="GA4" s="0"/>
+      <c r="GB4" s="0"/>
+      <c r="GC4" s="0"/>
+      <c r="GD4" s="0"/>
+      <c r="GE4" s="0"/>
+      <c r="GF4" s="0"/>
+      <c r="GG4" s="0"/>
+      <c r="GH4" s="0"/>
+      <c r="GI4" s="0"/>
+      <c r="GJ4" s="0"/>
+      <c r="GK4" s="0"/>
+      <c r="GL4" s="0"/>
+      <c r="GM4" s="0"/>
+      <c r="GN4" s="0"/>
+      <c r="GO4" s="0"/>
+      <c r="GP4" s="0"/>
+      <c r="GQ4" s="0"/>
+      <c r="GR4" s="0"/>
+      <c r="GS4" s="0"/>
+      <c r="GT4" s="0"/>
+      <c r="GU4" s="0"/>
+      <c r="GV4" s="0"/>
+      <c r="GW4" s="0"/>
+      <c r="GX4" s="0"/>
+      <c r="GY4" s="0"/>
+      <c r="GZ4" s="0"/>
+      <c r="HA4" s="0"/>
+      <c r="HB4" s="0"/>
+      <c r="HC4" s="0"/>
+      <c r="HD4" s="0"/>
+      <c r="HE4" s="0"/>
+      <c r="HF4" s="0"/>
+      <c r="HG4" s="0"/>
+      <c r="HH4" s="0"/>
+      <c r="HI4" s="0"/>
+      <c r="HJ4" s="0"/>
+      <c r="HK4" s="0"/>
+      <c r="HL4" s="0"/>
+      <c r="HM4" s="0"/>
+      <c r="HN4" s="0"/>
+      <c r="HO4" s="0"/>
+      <c r="HP4" s="0"/>
+      <c r="HQ4" s="0"/>
+      <c r="HR4" s="0"/>
+      <c r="HS4" s="0"/>
+      <c r="HT4" s="0"/>
+      <c r="HU4" s="0"/>
+      <c r="HV4" s="0"/>
+      <c r="HW4" s="0"/>
+      <c r="HX4" s="0"/>
+      <c r="HY4" s="0"/>
+      <c r="HZ4" s="0"/>
+      <c r="IA4" s="0"/>
+      <c r="IB4" s="0"/>
+      <c r="IC4" s="0"/>
+      <c r="ID4" s="0"/>
+      <c r="IE4" s="0"/>
+      <c r="IF4" s="0"/>
+      <c r="IG4" s="0"/>
+      <c r="IH4" s="0"/>
+      <c r="II4" s="0"/>
+      <c r="IJ4" s="0"/>
+      <c r="IK4" s="0"/>
+      <c r="IL4" s="0"/>
+      <c r="IM4" s="0"/>
+      <c r="IN4" s="0"/>
+      <c r="IO4" s="0"/>
+      <c r="IP4" s="0"/>
+      <c r="IQ4" s="0"/>
+      <c r="IR4" s="0"/>
+      <c r="IS4" s="0"/>
+      <c r="IT4" s="0"/>
+      <c r="IU4" s="0"/>
+      <c r="IV4" s="0"/>
+      <c r="IW4" s="0"/>
+      <c r="IX4" s="0"/>
+      <c r="IY4" s="0"/>
+      <c r="IZ4" s="0"/>
+      <c r="JA4" s="0"/>
+      <c r="JB4" s="0"/>
+      <c r="JC4" s="0"/>
+      <c r="JD4" s="0"/>
+      <c r="JE4" s="0"/>
+      <c r="JF4" s="0"/>
+      <c r="JG4" s="0"/>
+      <c r="JH4" s="0"/>
+      <c r="JI4" s="0"/>
+      <c r="JJ4" s="0"/>
+      <c r="JK4" s="0"/>
+      <c r="JL4" s="0"/>
+      <c r="JM4" s="0"/>
+      <c r="JN4" s="0"/>
+      <c r="JO4" s="0"/>
+      <c r="JP4" s="0"/>
+      <c r="JQ4" s="0"/>
+      <c r="JR4" s="0"/>
+      <c r="JS4" s="0"/>
+      <c r="JT4" s="0"/>
+      <c r="JU4" s="0"/>
+      <c r="JV4" s="0"/>
+      <c r="JW4" s="0"/>
+      <c r="JX4" s="0"/>
+      <c r="JY4" s="0"/>
+      <c r="JZ4" s="0"/>
+      <c r="KA4" s="0"/>
+      <c r="KB4" s="0"/>
+      <c r="KC4" s="0"/>
+      <c r="KD4" s="0"/>
+      <c r="KE4" s="0"/>
+      <c r="KF4" s="0"/>
+      <c r="KG4" s="0"/>
+      <c r="KH4" s="0"/>
+      <c r="KI4" s="0"/>
+      <c r="KJ4" s="0"/>
+      <c r="KK4" s="0"/>
+      <c r="KL4" s="0"/>
+      <c r="KM4" s="0"/>
+      <c r="KN4" s="0"/>
+      <c r="KO4" s="0"/>
+      <c r="KP4" s="0"/>
+      <c r="KQ4" s="0"/>
+      <c r="KR4" s="0"/>
+      <c r="KS4" s="0"/>
+      <c r="KT4" s="0"/>
+      <c r="KU4" s="0"/>
+      <c r="KV4" s="0"/>
+      <c r="KW4" s="0"/>
+      <c r="KX4" s="0"/>
+      <c r="KY4" s="0"/>
+      <c r="KZ4" s="0"/>
+      <c r="LA4" s="0"/>
+      <c r="LB4" s="0"/>
+      <c r="LC4" s="0"/>
+      <c r="LD4" s="0"/>
+      <c r="LE4" s="0"/>
+      <c r="LF4" s="0"/>
+      <c r="LG4" s="0"/>
+      <c r="LH4" s="0"/>
+      <c r="LI4" s="0"/>
+      <c r="LJ4" s="0"/>
+      <c r="LK4" s="0"/>
+      <c r="LL4" s="0"/>
+      <c r="LM4" s="0"/>
+      <c r="LN4" s="0"/>
+      <c r="LO4" s="0"/>
+      <c r="LP4" s="0"/>
+      <c r="LQ4" s="0"/>
+      <c r="LR4" s="0"/>
+      <c r="LS4" s="0"/>
+      <c r="LT4" s="0"/>
+      <c r="LU4" s="0"/>
+      <c r="LV4" s="0"/>
+      <c r="LW4" s="0"/>
+      <c r="LX4" s="0"/>
+      <c r="LY4" s="0"/>
+      <c r="LZ4" s="0"/>
+      <c r="MA4" s="0"/>
+      <c r="MB4" s="0"/>
+      <c r="MC4" s="0"/>
+      <c r="MD4" s="0"/>
+      <c r="ME4" s="0"/>
+      <c r="MF4" s="0"/>
+      <c r="MG4" s="0"/>
+      <c r="MH4" s="0"/>
+      <c r="MI4" s="0"/>
+      <c r="MJ4" s="0"/>
+      <c r="MK4" s="0"/>
+      <c r="ML4" s="0"/>
+      <c r="MM4" s="0"/>
+      <c r="MN4" s="0"/>
+      <c r="MO4" s="0"/>
+      <c r="MP4" s="0"/>
+      <c r="MQ4" s="0"/>
+      <c r="MR4" s="0"/>
+      <c r="MS4" s="0"/>
+      <c r="MT4" s="0"/>
+      <c r="MU4" s="0"/>
+      <c r="MV4" s="0"/>
+      <c r="MW4" s="0"/>
+      <c r="MX4" s="0"/>
+      <c r="MY4" s="0"/>
+      <c r="MZ4" s="0"/>
+      <c r="NA4" s="0"/>
+      <c r="NB4" s="0"/>
+      <c r="NC4" s="0"/>
+      <c r="ND4" s="0"/>
+      <c r="NE4" s="0"/>
+      <c r="NF4" s="0"/>
+      <c r="NG4" s="0"/>
+      <c r="NH4" s="0"/>
+      <c r="NI4" s="0"/>
+      <c r="NJ4" s="0"/>
+      <c r="NK4" s="0"/>
+      <c r="NL4" s="0"/>
+      <c r="NM4" s="0"/>
+      <c r="NN4" s="0"/>
+      <c r="NO4" s="0"/>
+      <c r="NP4" s="0"/>
+      <c r="NQ4" s="0"/>
+      <c r="NR4" s="0"/>
+      <c r="NS4" s="0"/>
+      <c r="NT4" s="0"/>
+      <c r="NU4" s="0"/>
+      <c r="NV4" s="0"/>
+      <c r="NW4" s="0"/>
+      <c r="NX4" s="0"/>
+      <c r="NY4" s="0"/>
+      <c r="NZ4" s="0"/>
+      <c r="OA4" s="0"/>
+      <c r="OB4" s="0"/>
+      <c r="OC4" s="0"/>
+      <c r="OD4" s="0"/>
+      <c r="OE4" s="0"/>
+      <c r="OF4" s="0"/>
+      <c r="OG4" s="0"/>
+      <c r="OH4" s="0"/>
+      <c r="OI4" s="0"/>
+      <c r="OJ4" s="0"/>
+      <c r="OK4" s="0"/>
+      <c r="OL4" s="0"/>
+      <c r="OM4" s="0"/>
+      <c r="ON4" s="0"/>
+      <c r="OO4" s="0"/>
+      <c r="OP4" s="0"/>
+      <c r="OQ4" s="0"/>
+      <c r="OR4" s="0"/>
+      <c r="OS4" s="0"/>
+      <c r="OT4" s="0"/>
+      <c r="OU4" s="0"/>
+      <c r="OV4" s="0"/>
+      <c r="OW4" s="0"/>
+      <c r="OX4" s="0"/>
+      <c r="OY4" s="0"/>
+      <c r="OZ4" s="0"/>
+      <c r="PA4" s="0"/>
+      <c r="PB4" s="0"/>
+      <c r="PC4" s="0"/>
+      <c r="PD4" s="0"/>
+      <c r="PE4" s="0"/>
+      <c r="PF4" s="0"/>
+      <c r="PG4" s="0"/>
+      <c r="PH4" s="0"/>
+      <c r="PI4" s="0"/>
+      <c r="PJ4" s="0"/>
+      <c r="PK4" s="0"/>
+      <c r="PL4" s="0"/>
+      <c r="PM4" s="0"/>
+      <c r="PN4" s="0"/>
+      <c r="PO4" s="0"/>
+      <c r="PP4" s="0"/>
+      <c r="PQ4" s="0"/>
+      <c r="PR4" s="0"/>
+      <c r="PS4" s="0"/>
+      <c r="PT4" s="0"/>
+      <c r="PU4" s="0"/>
+      <c r="PV4" s="0"/>
+      <c r="PW4" s="0"/>
+      <c r="PX4" s="0"/>
+      <c r="PY4" s="0"/>
+      <c r="PZ4" s="0"/>
+      <c r="QA4" s="0"/>
+      <c r="QB4" s="0"/>
+      <c r="QC4" s="0"/>
+      <c r="QD4" s="0"/>
+      <c r="QE4" s="0"/>
+      <c r="QF4" s="0"/>
+      <c r="QG4" s="0"/>
+      <c r="QH4" s="0"/>
+      <c r="QI4" s="0"/>
+      <c r="QJ4" s="0"/>
+      <c r="QK4" s="0"/>
+      <c r="QL4" s="0"/>
+      <c r="QM4" s="0"/>
+      <c r="QN4" s="0"/>
+      <c r="QO4" s="0"/>
+      <c r="QP4" s="0"/>
+      <c r="QQ4" s="0"/>
+      <c r="QR4" s="0"/>
+      <c r="QS4" s="0"/>
+      <c r="QT4" s="0"/>
+      <c r="QU4" s="0"/>
+      <c r="QV4" s="0"/>
+      <c r="QW4" s="0"/>
+      <c r="QX4" s="0"/>
+      <c r="QY4" s="0"/>
+      <c r="QZ4" s="0"/>
+      <c r="RA4" s="0"/>
+      <c r="RB4" s="0"/>
+      <c r="RC4" s="0"/>
+      <c r="RD4" s="0"/>
+      <c r="RE4" s="0"/>
+      <c r="RF4" s="0"/>
+      <c r="RG4" s="0"/>
+      <c r="RH4" s="0"/>
+      <c r="RI4" s="0"/>
+      <c r="RJ4" s="0"/>
+      <c r="RK4" s="0"/>
+      <c r="RL4" s="0"/>
+      <c r="RM4" s="0"/>
+      <c r="RN4" s="0"/>
+      <c r="RO4" s="0"/>
+      <c r="RP4" s="0"/>
+      <c r="RQ4" s="0"/>
+      <c r="RR4" s="0"/>
+      <c r="RS4" s="0"/>
+      <c r="RT4" s="0"/>
+      <c r="RU4" s="0"/>
+      <c r="RV4" s="0"/>
+      <c r="RW4" s="0"/>
+      <c r="RX4" s="0"/>
+      <c r="RY4" s="0"/>
+      <c r="RZ4" s="0"/>
+      <c r="SA4" s="0"/>
+      <c r="SB4" s="0"/>
+      <c r="SC4" s="0"/>
+      <c r="SD4" s="0"/>
+      <c r="SE4" s="0"/>
+      <c r="SF4" s="0"/>
+      <c r="SG4" s="0"/>
+      <c r="SH4" s="0"/>
+      <c r="SI4" s="0"/>
+      <c r="SJ4" s="0"/>
+      <c r="SK4" s="0"/>
+      <c r="SL4" s="0"/>
+      <c r="SM4" s="0"/>
+      <c r="SN4" s="0"/>
+      <c r="SO4" s="0"/>
+      <c r="SP4" s="0"/>
+      <c r="SQ4" s="0"/>
+      <c r="SR4" s="0"/>
+      <c r="SS4" s="0"/>
+      <c r="ST4" s="0"/>
+      <c r="SU4" s="0"/>
+      <c r="SV4" s="0"/>
+      <c r="SW4" s="0"/>
+      <c r="SX4" s="0"/>
+      <c r="SY4" s="0"/>
+      <c r="SZ4" s="0"/>
+      <c r="TA4" s="0"/>
+      <c r="TB4" s="0"/>
+      <c r="TC4" s="0"/>
+      <c r="TD4" s="0"/>
+      <c r="TE4" s="0"/>
+      <c r="TF4" s="0"/>
+      <c r="TG4" s="0"/>
+      <c r="TH4" s="0"/>
+      <c r="TI4" s="0"/>
+      <c r="TJ4" s="0"/>
+      <c r="TK4" s="0"/>
+      <c r="TL4" s="0"/>
+      <c r="TM4" s="0"/>
+      <c r="TN4" s="0"/>
+      <c r="TO4" s="0"/>
+      <c r="TP4" s="0"/>
+      <c r="TQ4" s="0"/>
+      <c r="TR4" s="0"/>
+      <c r="TS4" s="0"/>
+      <c r="TT4" s="0"/>
+      <c r="TU4" s="0"/>
+      <c r="TV4" s="0"/>
+      <c r="TW4" s="0"/>
+      <c r="TX4" s="0"/>
+      <c r="TY4" s="0"/>
+      <c r="TZ4" s="0"/>
+      <c r="UA4" s="0"/>
+      <c r="UB4" s="0"/>
+      <c r="UC4" s="0"/>
+      <c r="UD4" s="0"/>
+      <c r="UE4" s="0"/>
+      <c r="UF4" s="0"/>
+      <c r="UG4" s="0"/>
+      <c r="UH4" s="0"/>
+      <c r="UI4" s="0"/>
+      <c r="UJ4" s="0"/>
+      <c r="UK4" s="0"/>
+      <c r="UL4" s="0"/>
+      <c r="UM4" s="0"/>
+      <c r="UN4" s="0"/>
+      <c r="UO4" s="0"/>
+      <c r="UP4" s="0"/>
+      <c r="UQ4" s="0"/>
+      <c r="UR4" s="0"/>
+      <c r="US4" s="0"/>
+      <c r="UT4" s="0"/>
+      <c r="UU4" s="0"/>
+      <c r="UV4" s="0"/>
+      <c r="UW4" s="0"/>
+      <c r="UX4" s="0"/>
+      <c r="UY4" s="0"/>
+      <c r="UZ4" s="0"/>
+      <c r="VA4" s="0"/>
+      <c r="VB4" s="0"/>
+      <c r="VC4" s="0"/>
+      <c r="VD4" s="0"/>
+      <c r="VE4" s="0"/>
+      <c r="VF4" s="0"/>
+      <c r="VG4" s="0"/>
+      <c r="VH4" s="0"/>
+      <c r="VI4" s="0"/>
+      <c r="VJ4" s="0"/>
+      <c r="VK4" s="0"/>
+      <c r="VL4" s="0"/>
+      <c r="VM4" s="0"/>
+      <c r="VN4" s="0"/>
+      <c r="VO4" s="0"/>
+      <c r="VP4" s="0"/>
+      <c r="VQ4" s="0"/>
+      <c r="VR4" s="0"/>
+      <c r="VS4" s="0"/>
+      <c r="VT4" s="0"/>
+      <c r="VU4" s="0"/>
+      <c r="VV4" s="0"/>
+      <c r="VW4" s="0"/>
+      <c r="VX4" s="0"/>
+      <c r="VY4" s="0"/>
+      <c r="VZ4" s="0"/>
+      <c r="WA4" s="0"/>
+      <c r="WB4" s="0"/>
+      <c r="WC4" s="0"/>
+      <c r="WD4" s="0"/>
+      <c r="WE4" s="0"/>
+      <c r="WF4" s="0"/>
+      <c r="WG4" s="0"/>
+      <c r="WH4" s="0"/>
+      <c r="WI4" s="0"/>
+      <c r="WJ4" s="0"/>
+      <c r="WK4" s="0"/>
+      <c r="WL4" s="0"/>
+      <c r="WM4" s="0"/>
+      <c r="WN4" s="0"/>
+      <c r="WO4" s="0"/>
+      <c r="WP4" s="0"/>
+      <c r="WQ4" s="0"/>
+      <c r="WR4" s="0"/>
+      <c r="WS4" s="0"/>
+      <c r="WT4" s="0"/>
+      <c r="WU4" s="0"/>
+      <c r="WV4" s="0"/>
+      <c r="WW4" s="0"/>
+      <c r="WX4" s="0"/>
+      <c r="WY4" s="0"/>
+      <c r="WZ4" s="0"/>
+      <c r="XA4" s="0"/>
+      <c r="XB4" s="0"/>
+      <c r="XC4" s="0"/>
+      <c r="XD4" s="0"/>
+      <c r="XE4" s="0"/>
+      <c r="XF4" s="0"/>
+      <c r="XG4" s="0"/>
+      <c r="XH4" s="0"/>
+      <c r="XI4" s="0"/>
+      <c r="XJ4" s="0"/>
+      <c r="XK4" s="0"/>
+      <c r="XL4" s="0"/>
+      <c r="XM4" s="0"/>
+      <c r="XN4" s="0"/>
+      <c r="XO4" s="0"/>
+      <c r="XP4" s="0"/>
+      <c r="XQ4" s="0"/>
+      <c r="XR4" s="0"/>
+      <c r="XS4" s="0"/>
+      <c r="XT4" s="0"/>
+      <c r="XU4" s="0"/>
+      <c r="XV4" s="0"/>
+      <c r="XW4" s="0"/>
+      <c r="XX4" s="0"/>
+      <c r="XY4" s="0"/>
+      <c r="XZ4" s="0"/>
+      <c r="YA4" s="0"/>
+      <c r="YB4" s="0"/>
+      <c r="YC4" s="0"/>
+      <c r="YD4" s="0"/>
+      <c r="YE4" s="0"/>
+      <c r="YF4" s="0"/>
+      <c r="YG4" s="0"/>
+      <c r="YH4" s="0"/>
+      <c r="YI4" s="0"/>
+      <c r="YJ4" s="0"/>
+      <c r="YK4" s="0"/>
+      <c r="YL4" s="0"/>
+      <c r="YM4" s="0"/>
+      <c r="YN4" s="0"/>
+      <c r="YO4" s="0"/>
+      <c r="YP4" s="0"/>
+      <c r="YQ4" s="0"/>
+      <c r="YR4" s="0"/>
+      <c r="YS4" s="0"/>
+      <c r="YT4" s="0"/>
+      <c r="YU4" s="0"/>
+      <c r="YV4" s="0"/>
+      <c r="YW4" s="0"/>
+      <c r="YX4" s="0"/>
+      <c r="YY4" s="0"/>
+      <c r="YZ4" s="0"/>
+      <c r="ZA4" s="0"/>
+      <c r="ZB4" s="0"/>
+      <c r="ZC4" s="0"/>
+      <c r="ZD4" s="0"/>
+      <c r="ZE4" s="0"/>
+      <c r="ZF4" s="0"/>
+      <c r="ZG4" s="0"/>
+      <c r="ZH4" s="0"/>
+      <c r="ZI4" s="0"/>
+      <c r="ZJ4" s="0"/>
+      <c r="ZK4" s="0"/>
+      <c r="ZL4" s="0"/>
+      <c r="ZM4" s="0"/>
+      <c r="ZN4" s="0"/>
+      <c r="ZO4" s="0"/>
+      <c r="ZP4" s="0"/>
+      <c r="ZQ4" s="0"/>
+      <c r="ZR4" s="0"/>
+      <c r="ZS4" s="0"/>
+      <c r="ZT4" s="0"/>
+      <c r="ZU4" s="0"/>
+      <c r="ZV4" s="0"/>
+      <c r="ZW4" s="0"/>
+      <c r="ZX4" s="0"/>
+      <c r="ZY4" s="0"/>
+      <c r="ZZ4" s="0"/>
+      <c r="AAA4" s="0"/>
+      <c r="AAB4" s="0"/>
+      <c r="AAC4" s="0"/>
+      <c r="AAD4" s="0"/>
+      <c r="AAE4" s="0"/>
+      <c r="AAF4" s="0"/>
+      <c r="AAG4" s="0"/>
+      <c r="AAH4" s="0"/>
+      <c r="AAI4" s="0"/>
+      <c r="AAJ4" s="0"/>
+      <c r="AAK4" s="0"/>
+      <c r="AAL4" s="0"/>
+      <c r="AAM4" s="0"/>
+      <c r="AAN4" s="0"/>
+      <c r="AAO4" s="0"/>
+      <c r="AAP4" s="0"/>
+      <c r="AAQ4" s="0"/>
+      <c r="AAR4" s="0"/>
+      <c r="AAS4" s="0"/>
+      <c r="AAT4" s="0"/>
+      <c r="AAU4" s="0"/>
+      <c r="AAV4" s="0"/>
+      <c r="AAW4" s="0"/>
+      <c r="AAX4" s="0"/>
+      <c r="AAY4" s="0"/>
+      <c r="AAZ4" s="0"/>
+      <c r="ABA4" s="0"/>
+      <c r="ABB4" s="0"/>
+      <c r="ABC4" s="0"/>
+      <c r="ABD4" s="0"/>
+      <c r="ABE4" s="0"/>
+      <c r="ABF4" s="0"/>
+      <c r="ABG4" s="0"/>
+      <c r="ABH4" s="0"/>
+      <c r="ABI4" s="0"/>
+      <c r="ABJ4" s="0"/>
+      <c r="ABK4" s="0"/>
+      <c r="ABL4" s="0"/>
+      <c r="ABM4" s="0"/>
+      <c r="ABN4" s="0"/>
+      <c r="ABO4" s="0"/>
+      <c r="ABP4" s="0"/>
+      <c r="ABQ4" s="0"/>
+      <c r="ABR4" s="0"/>
+      <c r="ABS4" s="0"/>
+      <c r="ABT4" s="0"/>
+      <c r="ABU4" s="0"/>
+      <c r="ABV4" s="0"/>
+      <c r="ABW4" s="0"/>
+      <c r="ABX4" s="0"/>
+      <c r="ABY4" s="0"/>
+      <c r="ABZ4" s="0"/>
+      <c r="ACA4" s="0"/>
+      <c r="ACB4" s="0"/>
+      <c r="ACC4" s="0"/>
+      <c r="ACD4" s="0"/>
+      <c r="ACE4" s="0"/>
+      <c r="ACF4" s="0"/>
+      <c r="ACG4" s="0"/>
+      <c r="ACH4" s="0"/>
+      <c r="ACI4" s="0"/>
+      <c r="ACJ4" s="0"/>
+      <c r="ACK4" s="0"/>
+      <c r="ACL4" s="0"/>
+      <c r="ACM4" s="0"/>
+      <c r="ACN4" s="0"/>
+      <c r="ACO4" s="0"/>
+      <c r="ACP4" s="0"/>
+      <c r="ACQ4" s="0"/>
+      <c r="ACR4" s="0"/>
+      <c r="ACS4" s="0"/>
+      <c r="ACT4" s="0"/>
+      <c r="ACU4" s="0"/>
+      <c r="ACV4" s="0"/>
+      <c r="ACW4" s="0"/>
+      <c r="ACX4" s="0"/>
+      <c r="ACY4" s="0"/>
+      <c r="ACZ4" s="0"/>
+      <c r="ADA4" s="0"/>
+      <c r="ADB4" s="0"/>
+      <c r="ADC4" s="0"/>
+      <c r="ADD4" s="0"/>
+      <c r="ADE4" s="0"/>
+      <c r="ADF4" s="0"/>
+      <c r="ADG4" s="0"/>
+      <c r="ADH4" s="0"/>
+      <c r="ADI4" s="0"/>
+      <c r="ADJ4" s="0"/>
+      <c r="ADK4" s="0"/>
+      <c r="ADL4" s="0"/>
+      <c r="ADM4" s="0"/>
+      <c r="ADN4" s="0"/>
+      <c r="ADO4" s="0"/>
+      <c r="ADP4" s="0"/>
+      <c r="ADQ4" s="0"/>
+      <c r="ADR4" s="0"/>
+      <c r="ADS4" s="0"/>
+      <c r="ADT4" s="0"/>
+      <c r="ADU4" s="0"/>
+      <c r="ADV4" s="0"/>
+      <c r="ADW4" s="0"/>
+      <c r="ADX4" s="0"/>
+      <c r="ADY4" s="0"/>
+      <c r="ADZ4" s="0"/>
+      <c r="AEA4" s="0"/>
+      <c r="AEB4" s="0"/>
+      <c r="AEC4" s="0"/>
+      <c r="AED4" s="0"/>
+      <c r="AEE4" s="0"/>
+      <c r="AEF4" s="0"/>
+      <c r="AEG4" s="0"/>
+      <c r="AEH4" s="0"/>
+      <c r="AEI4" s="0"/>
+      <c r="AEJ4" s="0"/>
+      <c r="AEK4" s="0"/>
+      <c r="AEL4" s="0"/>
+      <c r="AEM4" s="0"/>
+      <c r="AEN4" s="0"/>
+      <c r="AEO4" s="0"/>
+      <c r="AEP4" s="0"/>
+      <c r="AEQ4" s="0"/>
+      <c r="AER4" s="0"/>
+      <c r="AES4" s="0"/>
+      <c r="AET4" s="0"/>
+      <c r="AEU4" s="0"/>
+      <c r="AEV4" s="0"/>
+      <c r="AEW4" s="0"/>
+      <c r="AEX4" s="0"/>
+      <c r="AEY4" s="0"/>
+      <c r="AEZ4" s="0"/>
+      <c r="AFA4" s="0"/>
+      <c r="AFB4" s="0"/>
+      <c r="AFC4" s="0"/>
+      <c r="AFD4" s="0"/>
+      <c r="AFE4" s="0"/>
+      <c r="AFF4" s="0"/>
+      <c r="AFG4" s="0"/>
+      <c r="AFH4" s="0"/>
+      <c r="AFI4" s="0"/>
+      <c r="AFJ4" s="0"/>
+      <c r="AFK4" s="0"/>
+      <c r="AFL4" s="0"/>
+      <c r="AFM4" s="0"/>
+      <c r="AFN4" s="0"/>
+      <c r="AFO4" s="0"/>
+      <c r="AFP4" s="0"/>
+      <c r="AFQ4" s="0"/>
+      <c r="AFR4" s="0"/>
+      <c r="AFS4" s="0"/>
+      <c r="AFT4" s="0"/>
+      <c r="AFU4" s="0"/>
+      <c r="AFV4" s="0"/>
+      <c r="AFW4" s="0"/>
+      <c r="AFX4" s="0"/>
+      <c r="AFY4" s="0"/>
+      <c r="AFZ4" s="0"/>
+      <c r="AGA4" s="0"/>
+      <c r="AGB4" s="0"/>
+      <c r="AGC4" s="0"/>
+      <c r="AGD4" s="0"/>
+      <c r="AGE4" s="0"/>
+      <c r="AGF4" s="0"/>
+      <c r="AGG4" s="0"/>
+      <c r="AGH4" s="0"/>
+      <c r="AGI4" s="0"/>
+      <c r="AGJ4" s="0"/>
+      <c r="AGK4" s="0"/>
+      <c r="AGL4" s="0"/>
+      <c r="AGM4" s="0"/>
+      <c r="AGN4" s="0"/>
+      <c r="AGO4" s="0"/>
+      <c r="AGP4" s="0"/>
+      <c r="AGQ4" s="0"/>
+      <c r="AGR4" s="0"/>
+      <c r="AGS4" s="0"/>
+      <c r="AGT4" s="0"/>
+      <c r="AGU4" s="0"/>
+      <c r="AGV4" s="0"/>
+      <c r="AGW4" s="0"/>
+      <c r="AGX4" s="0"/>
+      <c r="AGY4" s="0"/>
+      <c r="AGZ4" s="0"/>
+      <c r="AHA4" s="0"/>
+      <c r="AHB4" s="0"/>
+      <c r="AHC4" s="0"/>
+      <c r="AHD4" s="0"/>
+      <c r="AHE4" s="0"/>
+      <c r="AHF4" s="0"/>
+      <c r="AHG4" s="0"/>
+      <c r="AHH4" s="0"/>
+      <c r="AHI4" s="0"/>
+      <c r="AHJ4" s="0"/>
+      <c r="AHK4" s="0"/>
+      <c r="AHL4" s="0"/>
+      <c r="AHM4" s="0"/>
+      <c r="AHN4" s="0"/>
+      <c r="AHO4" s="0"/>
+      <c r="AHP4" s="0"/>
+      <c r="AHQ4" s="0"/>
+      <c r="AHR4" s="0"/>
+      <c r="AHS4" s="0"/>
+      <c r="AHT4" s="0"/>
+      <c r="AHU4" s="0"/>
+      <c r="AHV4" s="0"/>
+      <c r="AHW4" s="0"/>
+      <c r="AHX4" s="0"/>
+      <c r="AHY4" s="0"/>
+      <c r="AHZ4" s="0"/>
+      <c r="AIA4" s="0"/>
+      <c r="AIB4" s="0"/>
+      <c r="AIC4" s="0"/>
+      <c r="AID4" s="0"/>
+      <c r="AIE4" s="0"/>
+      <c r="AIF4" s="0"/>
+      <c r="AIG4" s="0"/>
+      <c r="AIH4" s="0"/>
+      <c r="AII4" s="0"/>
+      <c r="AIJ4" s="0"/>
+      <c r="AIK4" s="0"/>
+      <c r="AIL4" s="0"/>
+      <c r="AIM4" s="0"/>
+      <c r="AIN4" s="0"/>
+      <c r="AIO4" s="0"/>
+      <c r="AIP4" s="0"/>
+      <c r="AIQ4" s="0"/>
+      <c r="AIR4" s="0"/>
+      <c r="AIS4" s="0"/>
+      <c r="AIT4" s="0"/>
+      <c r="AIU4" s="0"/>
+      <c r="AIV4" s="0"/>
+      <c r="AIW4" s="0"/>
+      <c r="AIX4" s="0"/>
+      <c r="AIY4" s="0"/>
+      <c r="AIZ4" s="0"/>
+      <c r="AJA4" s="0"/>
+      <c r="AJB4" s="0"/>
+      <c r="AJC4" s="0"/>
+      <c r="AJD4" s="0"/>
+      <c r="AJE4" s="0"/>
+      <c r="AJF4" s="0"/>
+      <c r="AJG4" s="0"/>
+      <c r="AJH4" s="0"/>
+      <c r="AJI4" s="0"/>
+      <c r="AJJ4" s="0"/>
+      <c r="AJK4" s="0"/>
+      <c r="AJL4" s="0"/>
+      <c r="AJM4" s="0"/>
+      <c r="AJN4" s="0"/>
+      <c r="AJO4" s="0"/>
+      <c r="AJP4" s="0"/>
+      <c r="AJQ4" s="0"/>
+      <c r="AJR4" s="0"/>
+      <c r="AJS4" s="0"/>
+      <c r="AJT4" s="0"/>
+      <c r="AJU4" s="0"/>
+      <c r="AJV4" s="0"/>
+      <c r="AJW4" s="0"/>
+      <c r="AJX4" s="0"/>
+      <c r="AJY4" s="0"/>
+      <c r="AJZ4" s="0"/>
+      <c r="AKA4" s="0"/>
+      <c r="AKB4" s="0"/>
+      <c r="AKC4" s="0"/>
+      <c r="AKD4" s="0"/>
+      <c r="AKE4" s="0"/>
+      <c r="AKF4" s="0"/>
+      <c r="AKG4" s="0"/>
+      <c r="AKH4" s="0"/>
+      <c r="AKI4" s="0"/>
+      <c r="AKJ4" s="0"/>
+      <c r="AKK4" s="0"/>
+      <c r="AKL4" s="0"/>
+      <c r="AKM4" s="0"/>
+      <c r="AKN4" s="0"/>
+      <c r="AKO4" s="0"/>
+      <c r="AKP4" s="0"/>
+      <c r="AKQ4" s="0"/>
+      <c r="AKR4" s="0"/>
+      <c r="AKS4" s="0"/>
+      <c r="AKT4" s="0"/>
+      <c r="AKU4" s="0"/>
+      <c r="AKV4" s="0"/>
+      <c r="AKW4" s="0"/>
+      <c r="AKX4" s="0"/>
+      <c r="AKY4" s="0"/>
+      <c r="AKZ4" s="0"/>
+      <c r="ALA4" s="0"/>
+      <c r="ALB4" s="0"/>
+      <c r="ALC4" s="0"/>
+      <c r="ALD4" s="0"/>
+      <c r="ALE4" s="0"/>
+      <c r="ALF4" s="0"/>
+      <c r="ALG4" s="0"/>
+      <c r="ALH4" s="0"/>
+      <c r="ALI4" s="0"/>
+      <c r="ALJ4" s="0"/>
+      <c r="ALK4" s="0"/>
+      <c r="ALL4" s="0"/>
+      <c r="ALM4" s="0"/>
+      <c r="ALN4" s="0"/>
+      <c r="ALO4" s="0"/>
+      <c r="ALP4" s="0"/>
+      <c r="ALQ4" s="0"/>
+      <c r="ALR4" s="0"/>
+      <c r="ALS4" s="0"/>
+      <c r="ALT4" s="0"/>
+      <c r="ALU4" s="0"/>
+      <c r="ALV4" s="0"/>
+      <c r="ALW4" s="0"/>
+      <c r="ALX4" s="0"/>
+      <c r="ALY4" s="0"/>
+      <c r="ALZ4" s="0"/>
+      <c r="AMA4" s="0"/>
+      <c r="AMB4" s="0"/>
+      <c r="AMC4" s="0"/>
+      <c r="AMD4" s="0"/>
+      <c r="AME4" s="0"/>
+      <c r="AMF4" s="0"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E1" type="list">
@@ -3499,37 +4595,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="22.1255060728745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="35.2914979757085"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.7692307692308"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.4493927125506"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="19.6518218623482"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="15.1619433198381"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="93.1417004048583"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="31.7651821862348"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="10.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="23.5141700404858"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="37.5506072874494"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="22.2226720647773"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="16.1255060728745"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="53.3441295546559"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="33.7975708502024"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="11.085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>3</v>
@@ -3541,12 +4637,147 @@
         <v>7</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="66.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Few fixes for gpio wakeup
</commit_message>
<xml_diff>
--- a/doc/WOLFE_APB_SOC_CTRL_reference.xlsx
+++ b/doc/WOLFE_APB_SOC_CTRL_reference.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="47">
   <si>
     <t xml:space="preserve">Register Name</t>
   </si>
@@ -128,7 +128,7 @@
     <t xml:space="preserve">MEM_RET_0</t>
   </si>
   <si>
-    <t xml:space="preserve">Memory retention configuration.</t>
+    <t xml:space="preserve">Memory retention configuration part 0.</t>
   </si>
   <si>
     <t xml:space="preserve">EXTWAKEUP_SEL</t>
@@ -151,6 +151,30 @@
   </si>
   <si>
     <t xml:space="preserve">External wakeup enable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WAKEUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wake-up state. This specifies in which state the PMU should wakeup the chip.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOT_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boot type. This is a user field written by the SW which is interpreted by the oot code and runtime after the chip has rebooted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLUSTER_WAKEUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster wakeup state.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEM_RET_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory retention configuration part 1.</t>
   </si>
 </sst>
 </file>
@@ -377,18 +401,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.0485829959514"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.9878542510121"/>
     <col collapsed="false" hidden="true" max="2" min="2" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.51821862348178"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="11.085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.3400809716599"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="62.3441295546559"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="11.085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="2" width="11.085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="5.8421052631579"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.7692307692308"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="66.3643724696356"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="61.165991902834"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="2" width="11.7813765182186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4595,26 +4619,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="23.5141700404858"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="37.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="22.2226720647773"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="16.1255060728745"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="53.3441295546559"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="33.7975708502024"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="11.085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="39.9554655870445"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="23.6153846153846"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="22.2226720647773"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="56.7732793522267"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="11.7813765182186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4778,6 +4802,114 @@
         <v>38</v>
       </c>
       <c r="I6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>